<commit_message>
Updated Sender Form, added Sender ID Request features
</commit_message>
<xml_diff>
--- a/uploads/mysms/recipients_sample.xlsx
+++ b/uploads/mysms/recipients_sample.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4301CE-8F75-44B0-BD62-5E7F7A77A36A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="recipients" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
   <si>
     <t xml:space="preserve">NAME </t>
   </si>
@@ -80,12 +81,18 @@
   </si>
   <si>
     <t>Sms Recipient 20</t>
+  </si>
+  <si>
+    <t>GROUP</t>
+  </si>
+  <si>
+    <t>Grp1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -221,6 +228,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -256,6 +280,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -431,185 +472,249 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.90625" customWidth="1"/>
     <col min="2" max="2" width="17.36328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1">
         <v>255000000000</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1">
         <v>255000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1">
         <v>255000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1">
         <v>255000000003</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="1">
         <v>255000000004</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="1">
         <v>255000000005</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="1">
         <v>255000000006</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1">
         <v>255000000007</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="1">
         <v>255000000008</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="1">
         <v>255000000009</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="1">
         <v>255000000010</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="1">
         <v>255000000011</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="1">
         <v>255000000012</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="1">
         <v>255000000013</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="1">
         <v>255000000014</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="1">
         <v>255000000015</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="1">
         <v>255000000016</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="1">
         <v>255000000017</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="1">
         <v>255000000018</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="1">
         <v>255000000019</v>
+      </c>
+      <c r="C21" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>